<commit_message>
Inaugural Speeches Project Upload
</commit_message>
<xml_diff>
--- a/data/InaugurationInfo.xlsx
+++ b/data/InaugurationInfo.xlsx
@@ -1,34 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tianzheng/Dropbox/Tian_Teaching/G5243-ADS/Spring2017/Tutorials/speeches/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8080" yWindow="3420" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="91">
   <si>
     <t>President</t>
   </si>
@@ -154,9 +149,6 @@
   </si>
   <si>
     <t>Donald J. Trump</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>Term</t>
@@ -413,7 +405,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -468,7 +460,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -523,7 +515,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -578,7 +570,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -633,7 +625,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -688,7 +680,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -743,7 +735,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -798,7 +790,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -853,7 +845,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -908,7 +900,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -963,7 +955,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1018,7 +1010,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1073,7 +1065,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1128,7 +1120,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1183,7 +1175,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1238,7 +1230,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1293,7 +1285,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1348,7 +1340,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1403,7 +1395,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1458,7 +1450,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1513,7 +1505,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1568,7 +1560,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1623,7 +1615,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1678,7 +1670,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1733,7 +1725,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1788,7 +1780,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1843,7 +1835,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1898,7 +1890,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1953,7 +1945,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2008,7 +2000,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2063,7 +2055,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2118,7 +2110,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2173,7 +2165,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2228,7 +2220,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2283,7 +2275,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2338,7 +2330,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2393,7 +2385,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2448,7 +2440,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2503,7 +2495,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2558,7 +2550,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2613,7 +2605,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2668,7 +2660,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2723,7 +2715,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2778,7 +2770,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2833,7 +2825,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2888,7 +2880,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2943,7 +2935,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -2998,7 +2990,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3053,7 +3045,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3108,7 +3100,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3163,7 +3155,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3218,7 +3210,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3273,7 +3265,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3328,7 +3320,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3383,7 +3375,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3438,7 +3430,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3493,7 +3485,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3548,7 +3540,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3603,7 +3595,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3658,7 +3650,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3713,7 +3705,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3768,7 +3760,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3823,7 +3815,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3878,7 +3870,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3933,7 +3925,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -3988,7 +3980,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4043,7 +4035,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4098,7 +4090,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4153,7 +4145,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4208,7 +4200,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4263,7 +4255,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4318,7 +4310,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4373,7 +4365,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4428,7 +4420,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4483,7 +4475,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4538,7 +4530,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4593,7 +4585,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4648,7 +4640,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4703,7 +4695,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4758,7 +4750,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4813,7 +4805,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4868,7 +4860,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4923,7 +4915,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -4978,7 +4970,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5033,7 +5025,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5088,7 +5080,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5143,7 +5135,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5198,7 +5190,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5253,7 +5245,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5308,7 +5300,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5363,7 +5355,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5418,7 +5410,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5473,7 +5465,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5528,7 +5520,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5583,7 +5575,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5638,7 +5630,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5693,7 +5685,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5748,7 +5740,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5803,7 +5795,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5858,7 +5850,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5913,7 +5905,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -5968,7 +5960,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6023,7 +6015,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6078,7 +6070,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6133,7 +6125,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6188,7 +6180,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6243,7 +6235,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6298,7 +6290,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6353,7 +6345,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6408,7 +6400,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6463,7 +6455,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6518,7 +6510,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6573,7 +6565,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6628,7 +6620,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6683,7 +6675,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6738,7 +6730,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6798,7 +6790,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6853,7 +6845,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6908,7 +6900,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -6963,7 +6955,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7018,7 +7010,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7073,7 +7065,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7128,7 +7120,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7183,7 +7175,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7238,7 +7230,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7293,7 +7285,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7348,7 +7340,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7403,7 +7395,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7458,7 +7450,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7513,7 +7505,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7568,7 +7560,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7623,7 +7615,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7678,7 +7670,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7733,7 +7725,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7788,7 +7780,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7843,7 +7835,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7898,7 +7890,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -7953,7 +7945,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8008,7 +8000,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8063,7 +8055,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8118,7 +8110,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8173,7 +8165,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8228,7 +8220,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8283,7 +8275,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8338,7 +8330,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8393,7 +8385,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8448,7 +8440,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8503,7 +8495,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8558,7 +8550,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8613,7 +8605,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8668,7 +8660,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8723,7 +8715,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8778,7 +8770,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8833,7 +8825,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8888,7 +8880,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8943,7 +8935,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -8998,7 +8990,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9053,7 +9045,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9108,7 +9100,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9163,7 +9155,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9218,7 +9210,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9273,7 +9265,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9328,7 +9320,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9383,7 +9375,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9438,7 +9430,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9493,7 +9485,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9548,7 +9540,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9603,7 +9595,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9658,7 +9650,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9713,7 +9705,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9768,7 +9760,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9823,7 +9815,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9878,7 +9870,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9933,7 +9925,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -9988,7 +9980,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10043,7 +10035,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10098,7 +10090,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10153,7 +10145,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10208,7 +10200,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10263,7 +10255,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10318,7 +10310,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10373,7 +10365,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10428,7 +10420,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10483,7 +10475,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10538,7 +10530,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10593,7 +10585,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10648,7 +10640,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10703,7 +10695,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10758,7 +10750,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10813,7 +10805,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10868,7 +10860,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10923,7 +10915,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -10978,7 +10970,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11033,7 +11025,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11088,7 +11080,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11143,7 +11135,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11198,7 +11190,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11253,7 +11245,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11308,7 +11300,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11363,7 +11355,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11418,7 +11410,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11473,7 +11465,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11528,7 +11520,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11583,7 +11575,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11638,7 +11630,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11693,7 +11685,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11748,7 +11740,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11803,7 +11795,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11858,7 +11850,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11913,7 +11905,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -11968,7 +11960,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12023,7 +12015,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12078,7 +12070,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12133,7 +12125,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12188,7 +12180,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12243,7 +12235,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12298,7 +12290,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12353,7 +12345,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12408,7 +12400,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12463,7 +12455,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12518,7 +12510,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12573,7 +12565,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12628,7 +12620,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12683,7 +12675,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12738,7 +12730,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12793,7 +12785,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12848,7 +12840,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12903,7 +12895,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -12958,7 +12950,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -13013,7 +13005,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -13071,7 +13063,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -13106,7 +13098,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -13283,7 +13275,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13293,1024 +13285,1029 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2">
         <v>1431</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2">
         <v>2321</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2">
         <v>1730</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2">
         <v>2166</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2">
         <v>1177</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2">
         <v>1211</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2">
         <v>3375</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2">
         <v>4472</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2">
         <v>2915</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2">
         <v>1128</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2">
         <v>1176</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="2">
         <v>3843</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="2">
         <v>8460</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2">
         <v>4809</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="2">
         <v>1090</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="2">
         <v>3336</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="2">
         <v>2831</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="2">
         <v>3637</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" s="2">
         <v>700</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2">
         <v>1127</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="2">
         <v>1339</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="2">
         <v>2486</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" s="2">
         <v>2979</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="2">
         <v>1686</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="2">
         <v>4392</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" s="2">
         <v>3968</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" s="2">
         <v>2218</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E31" s="2">
         <v>984</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E32" s="2">
         <v>5434</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="2">
         <v>1704</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E34" s="2">
         <v>1526</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" s="2">
         <v>3329</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E36" s="2">
         <v>4055</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E37" s="2">
         <v>3672</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E38" s="2">
         <v>1880</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E39" s="2">
         <v>1808</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" s="1">
         <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" s="2">
         <v>1359</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="1">
         <v>4</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E41" s="2">
         <v>559</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E42" s="2">
         <v>2273</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E43" s="2">
         <v>2459</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C44" s="1">
         <v>2</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E44" s="2">
         <v>1658</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E45" s="2">
         <v>1366</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" s="1">
         <v>1</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E46" s="2">
         <v>1507</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" s="1">
         <v>1</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E47" s="2">
         <v>2128</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48" s="1">
         <v>2</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E48" s="2">
         <v>1803</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49" s="2">
         <v>1229</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="1">
         <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E50" s="2">
         <v>2427</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51" s="1">
         <v>2</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E51" s="2">
         <v>2561</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E52" s="2">
         <v>2320</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C53" s="1">
         <v>1</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E53" s="2">
         <v>1598</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" s="1">
         <v>2</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E54" s="2">
         <v>2155</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E55" s="2">
         <v>1592</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C56" s="1">
         <v>2</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E56" s="2">
         <v>2071</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C57" s="1">
         <v>1</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E57" s="2">
         <v>2395</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" s="1">
         <v>2</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E58" s="2">
         <v>2096</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C59" s="1">
         <v>1</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1455</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -14320,9 +14317,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>